<commit_message>
Code Version 13052020 10:55
</commit_message>
<xml_diff>
--- a/Prime_Job_Automation/Configuration/Lookups/PostBatchScriptFileLocation.xlsx
+++ b/Prime_Job_Automation/Configuration/Lookups/PostBatchScriptFileLocation.xlsx
@@ -5,35 +5,27 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Prime_Job_Automation\Configuration\Lookups\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\PJA\Prime_Job_Automation\Configuration\Lookups\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46242E34-AA21-493C-8FA5-641BF059A614}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBB5F635-1E4E-419A-9B03-233E8B598AF2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{3C0CB0ED-1A72-4CDA-B30F-C1DF2FE8AF9D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="23">
-  <si>
-    <t>ScriptPath</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
   <si>
     <t>/tsys/prime/UBP_ubp/datawarehouse_file/EDS_TRANSFER//TSYS_DW.sh</t>
   </si>
@@ -47,9 +39,6 @@
     <t>S.No</t>
   </si>
   <si>
-    <t>/home/pmuser01/move_reports.com</t>
-  </si>
-  <si>
     <t>/tsys/prime/deployment/CREDIT/GLConv</t>
   </si>
   <si>
@@ -59,64 +48,74 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>/tsys/prime/UBP_ubp/interfaces_outgoing/yyyymmdd</t>
-  </si>
-  <si>
-    <t>/tsys/prime/deployment/CREDIT/Emboss/Inputs</t>
-  </si>
-  <si>
     <t>/tsys/prime/deployment/CREDIT/Emboss/Work/runEmboss.com</t>
   </si>
   <si>
-    <t>/tsys/prime/deployment/CREDIT/Emboss/Outputs/NonEmbossing</t>
-  </si>
-  <si>
-    <t>/tsys/prime/deployment/CREDIT/Emboss/Outputs/Embossing/</t>
-  </si>
-  <si>
-    <t>/tsys/prime/UBP_ubp/statement_files</t>
-  </si>
-  <si>
-    <t>/tsys/prime/UBP_ubp/host_debit_files</t>
-  </si>
-  <si>
     <t>/tsys/prime/deployment/CREDIT/directdebit/in</t>
   </si>
   <si>
-    <t>/tsys/prime/deployment/CREDIT/directdebit/work/directdebit.sh</t>
-  </si>
-  <si>
     <t>/tsys/prime/deployment/CREDIT/directdebit/work//directdebit.com</t>
   </si>
   <si>
     <t>IsExist?</t>
   </si>
   <si>
-    <t>/tsys/prime/UBP_ubp/collector_outgoing_files/yyyymmdd</t>
-  </si>
-  <si>
-    <t>/tsys/prime/UBP_ubp/reports/yyyymmdd</t>
-  </si>
-  <si>
-    <t>/tsys/prime/UBP_ubp/gl/yyyymmdd</t>
+    <t>TSYSDW</t>
+  </si>
+  <si>
+    <t>MVReports</t>
+  </si>
+  <si>
+    <t>GLConv</t>
+  </si>
+  <si>
+    <t>GLBackup</t>
+  </si>
+  <si>
+    <t>RunEmboss</t>
+  </si>
+  <si>
+    <t>/tsys/prime/deployment/CREDIT/directdebit/out</t>
+  </si>
+  <si>
+    <t>DirectDebitIn</t>
+  </si>
+  <si>
+    <t>DirectDebitShell</t>
+  </si>
+  <si>
+    <t>DirectDebitOut</t>
+  </si>
+  <si>
+    <t>VisaVCF</t>
+  </si>
+  <si>
+    <t>GLCPROConv</t>
+  </si>
+  <si>
+    <t>/home/pmuser01/move_reports.sh</t>
+  </si>
+  <si>
+    <t>/tsys/prime/UBP_ubp/visa_vcf_file/YYYYMMDD@CD</t>
+  </si>
+  <si>
+    <t>/tsys/prime/deployment/CREDIT/GLConv/Backup/yyyymmdd@CD</t>
+  </si>
+  <si>
+    <t>Activity_Name</t>
+  </si>
+  <si>
+    <t>Path</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -129,8 +128,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="10"/>
-      <color rgb="FFFF0000"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -177,11 +177,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -495,261 +506,185 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{246483EE-5B76-4FBE-8385-6DD4D9B60105}">
-  <dimension ref="A1:D21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="67.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="85.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="D4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="2"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="C10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+      <c r="C11" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>8</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>9</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="2"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>10</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
-        <v>11</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D12" s="2"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <v>12</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" s="2"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>13</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="2"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
-        <v>14</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" s="2"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
-        <v>15</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" s="2"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
-        <v>16</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" s="2"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
-        <v>17</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D18" s="2"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
-        <v>18</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D19" s="2"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
+      <c r="E11" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Code Version 14052020 02:40
</commit_message>
<xml_diff>
--- a/Prime_Job_Automation/Configuration/Lookups/PostBatchScriptFileLocation.xlsx
+++ b/Prime_Job_Automation/Configuration/Lookups/PostBatchScriptFileLocation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\PJA\Prime_Job_Automation\Configuration\Lookups\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBB5F635-1E4E-419A-9B03-233E8B598AF2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC53EFF2-A424-4933-88E0-36978FC7548A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="51">
   <si>
     <t>/tsys/prime/UBP_ubp/datawarehouse_file/EDS_TRANSFER//TSYS_DW.sh</t>
   </si>
@@ -39,9 +39,6 @@
     <t>S.No</t>
   </si>
   <si>
-    <t>/tsys/prime/deployment/CREDIT/GLConv</t>
-  </si>
-  <si>
     <t>/tsys/prime/deployment/CREDIT/GLConv/GLCPROConv.com</t>
   </si>
   <si>
@@ -54,9 +51,6 @@
     <t>/tsys/prime/deployment/CREDIT/directdebit/in</t>
   </si>
   <si>
-    <t>/tsys/prime/deployment/CREDIT/directdebit/work//directdebit.com</t>
-  </si>
-  <si>
     <t>IsExist?</t>
   </si>
   <si>
@@ -96,16 +90,94 @@
     <t>/home/pmuser01/move_reports.sh</t>
   </si>
   <si>
-    <t>/tsys/prime/UBP_ubp/visa_vcf_file/YYYYMMDD@CD</t>
-  </si>
-  <si>
-    <t>/tsys/prime/deployment/CREDIT/GLConv/Backup/yyyymmdd@CD</t>
-  </si>
-  <si>
     <t>Activity_Name</t>
   </si>
   <si>
     <t>Path</t>
+  </si>
+  <si>
+    <t>InterfaceOutgoing</t>
+  </si>
+  <si>
+    <t>/tsys/prime/UBP_ubp/interfaces_outgoing/</t>
+  </si>
+  <si>
+    <t>/tsys/prime/UBP_ubp/collector_outgoing_files/</t>
+  </si>
+  <si>
+    <t>Reports</t>
+  </si>
+  <si>
+    <t>/tsys/prime/UBP_ubp/reports/</t>
+  </si>
+  <si>
+    <t>GLCurrDate</t>
+  </si>
+  <si>
+    <t>/tsys/prime/UBP_ubp/gl/</t>
+  </si>
+  <si>
+    <t>EmbossInput</t>
+  </si>
+  <si>
+    <t>NonEmbossOutput</t>
+  </si>
+  <si>
+    <t>/tsys/prime/deployment/CREDIT/Emboss/Outputs/NonEmbossing/</t>
+  </si>
+  <si>
+    <t>EmbossOutput</t>
+  </si>
+  <si>
+    <t>/tsys/prime/deployment/CREDIT/Emboss/Outputs/Embossing/</t>
+  </si>
+  <si>
+    <t>StatementFiles</t>
+  </si>
+  <si>
+    <t>/tsys/prime/UBP_ubp/statement_files/</t>
+  </si>
+  <si>
+    <t>HostDebitFiles</t>
+  </si>
+  <si>
+    <t>/tsys/prime/UBP_ubp/host_debit_files/</t>
+  </si>
+  <si>
+    <t>ChckReports</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /home/pmuser01/check_reports.com</t>
+  </si>
+  <si>
+    <t>UBPEmbossFiles</t>
+  </si>
+  <si>
+    <t>/tsys/prime/UBP_ubp/embossing_files/</t>
+  </si>
+  <si>
+    <t>/tsys/prime/UBP_ubp/visa_vcf_file/</t>
+  </si>
+  <si>
+    <t>CollectorOutgoing</t>
+  </si>
+  <si>
+    <t>/tsys/prime/deployment/CREDIT/GLConv/Backup/</t>
+  </si>
+  <si>
+    <t>/tsys/prime/deployment/CREDIT/GLConv/</t>
+  </si>
+  <si>
+    <t>ConvertorOutput</t>
+  </si>
+  <si>
+    <t>/home/pmuser01/converters/convert_biller/work/convert_output.com</t>
+  </si>
+  <si>
+    <t>/tsys/prime/deployment/CREDIT/Emboss/Inputs/</t>
+  </si>
+  <si>
+    <t>/tsys/prime/deployment/CREDIT/directdebit/work/directdebit.com</t>
   </si>
 </sst>
 </file>
@@ -177,7 +249,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -193,6 +265,8 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -507,7 +581,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -524,16 +598,16 @@
         <v>3</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -541,7 +615,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>0</v>
@@ -556,10 +630,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>2</v>
@@ -571,13 +645,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E4" s="1"/>
     </row>
@@ -586,13 +660,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E5" s="1"/>
     </row>
@@ -601,13 +675,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E6" s="1"/>
     </row>
@@ -616,13 +690,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E7" s="1"/>
     </row>
@@ -631,13 +705,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E8" s="1"/>
     </row>
@@ -646,13 +720,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E9" s="1"/>
     </row>
@@ -661,13 +735,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E10" s="1"/>
     </row>
@@ -676,15 +750,195 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="9"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="9"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="9"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" s="9"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" s="9"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>17</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" s="9"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>18</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" s="9"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>19</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" s="9"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
         <v>20</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="B20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" s="9"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>21</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" s="9"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>22</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" s="9"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
         <v>23</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" s="1"/>
+      <c r="B23" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E23" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Code Version 15052020 00:25
</commit_message>
<xml_diff>
--- a/Prime_Job_Automation/Configuration/Lookups/PostBatchScriptFileLocation.xlsx
+++ b/Prime_Job_Automation/Configuration/Lookups/PostBatchScriptFileLocation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\PJA\Prime_Job_Automation\Configuration\Lookups\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC53EFF2-A424-4933-88E0-36978FC7548A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FC72857-FD93-48DB-92C1-0B0211508D84}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -642,28 +642,28 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>24</v>
+        <v>39</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>40</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="E4" s="9"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>5</v>
@@ -672,13 +672,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>5</v>
@@ -687,13 +687,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>5</v>
@@ -702,13 +702,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>5</v>
@@ -717,73 +717,73 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>4</v>
+        <v>28</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>49</v>
+        <v>19</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>4</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>10</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>6</v>
+        <v>9</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>49</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>11</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>32</v>
+        <v>10</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>6</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" s="9"/>
+        <v>2</v>
+      </c>
+      <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>5</v>
@@ -792,13 +792,13 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>5</v>
@@ -807,13 +807,13 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>5</v>
@@ -822,13 +822,13 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>5</v>
@@ -837,28 +837,28 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E17" s="9"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
Code Version 17052020 01:12
</commit_message>
<xml_diff>
--- a/Prime_Job_Automation/Configuration/Lookups/PostBatchScriptFileLocation.xlsx
+++ b/Prime_Job_Automation/Configuration/Lookups/PostBatchScriptFileLocation.xlsx
@@ -8,17 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\PJA\Prime_Job_Automation\Configuration\Lookups\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FC72857-FD93-48DB-92C1-0B0211508D84}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33F57BCB-920B-4C7F-8D2C-557FAE6AA6FF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>

</xml_diff>

<commit_message>
Code Version 18052020 17:45
</commit_message>
<xml_diff>
--- a/Prime_Job_Automation/Configuration/Lookups/PostBatchScriptFileLocation.xlsx
+++ b/Prime_Job_Automation/Configuration/Lookups/PostBatchScriptFileLocation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\PJA\Prime_Job_Automation\Configuration\Lookups\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33F57BCB-920B-4C7F-8D2C-557FAE6AA6FF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15AC5643-976D-43F2-96A1-065ED2E62921}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,9 +32,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="51">
   <si>
-    <t>/tsys/prime/UBP_ubp/datawarehouse_file/EDS_TRANSFER//TSYS_DW.sh</t>
-  </si>
-  <si>
     <t>IsFolder?</t>
   </si>
   <si>
@@ -53,9 +50,6 @@
     <t>/tsys/prime/deployment/CREDIT/Emboss/Work/runEmboss.com</t>
   </si>
   <si>
-    <t>/tsys/prime/deployment/CREDIT/directdebit/in</t>
-  </si>
-  <si>
     <t>IsExist?</t>
   </si>
   <si>
@@ -74,9 +68,6 @@
     <t>RunEmboss</t>
   </si>
   <si>
-    <t>/tsys/prime/deployment/CREDIT/directdebit/out</t>
-  </si>
-  <si>
     <t>DirectDebitIn</t>
   </si>
   <si>
@@ -92,9 +83,6 @@
     <t>GLCPROConv</t>
   </si>
   <si>
-    <t>/home/pmuser01/move_reports.sh</t>
-  </si>
-  <si>
     <t>Activity_Name</t>
   </si>
   <si>
@@ -104,24 +92,12 @@
     <t>InterfaceOutgoing</t>
   </si>
   <si>
-    <t>/tsys/prime/UBP_ubp/interfaces_outgoing/</t>
-  </si>
-  <si>
-    <t>/tsys/prime/UBP_ubp/collector_outgoing_files/</t>
-  </si>
-  <si>
     <t>Reports</t>
   </si>
   <si>
-    <t>/tsys/prime/UBP_ubp/reports/</t>
-  </si>
-  <si>
     <t>GLCurrDate</t>
   </si>
   <si>
-    <t>/tsys/prime/UBP_ubp/gl/</t>
-  </si>
-  <si>
     <t>EmbossInput</t>
   </si>
   <si>
@@ -140,36 +116,18 @@
     <t>StatementFiles</t>
   </si>
   <si>
-    <t>/tsys/prime/UBP_ubp/statement_files/</t>
-  </si>
-  <si>
     <t>HostDebitFiles</t>
   </si>
   <si>
-    <t>/tsys/prime/UBP_ubp/host_debit_files/</t>
-  </si>
-  <si>
     <t>ChckReports</t>
   </si>
   <si>
-    <t xml:space="preserve"> /home/pmuser01/check_reports.com</t>
-  </si>
-  <si>
     <t>UBPEmbossFiles</t>
   </si>
   <si>
-    <t>/tsys/prime/UBP_ubp/embossing_files/</t>
-  </si>
-  <si>
-    <t>/tsys/prime/UBP_ubp/visa_vcf_file/</t>
-  </si>
-  <si>
     <t>CollectorOutgoing</t>
   </si>
   <si>
-    <t>/tsys/prime/deployment/CREDIT/GLConv/Backup/</t>
-  </si>
-  <si>
     <t>/tsys/prime/deployment/CREDIT/GLConv/</t>
   </si>
   <si>
@@ -183,6 +141,48 @@
   </si>
   <si>
     <t>/tsys/prime/deployment/CREDIT/directdebit/work/directdebit.com</t>
+  </si>
+  <si>
+    <t>/home/pmuser01/check_reports.com</t>
+  </si>
+  <si>
+    <t>/prime/UBP_ubp/datawarehouse_file/EDS_TRANSFER//TSYS_DW.sh</t>
+  </si>
+  <si>
+    <t>/prime/UBP_ubp/interfaces_outgoing/</t>
+  </si>
+  <si>
+    <t>/prime/UBP_ubp/collector_outgoing_files/</t>
+  </si>
+  <si>
+    <t>/prime/UBP_ubp/reports/</t>
+  </si>
+  <si>
+    <t>/prime/UBP_ubp/gl/</t>
+  </si>
+  <si>
+    <t>/prime/UBP_ubp/statement_files/</t>
+  </si>
+  <si>
+    <t>/prime/UBP_ubp/host_debit_files/</t>
+  </si>
+  <si>
+    <t>/prime/UBP_ubp/embossing_files/</t>
+  </si>
+  <si>
+    <t>/prime/UBP_ubp/visa_vcf_file/</t>
+  </si>
+  <si>
+    <t>/home/pmuser01/MOVE_Reports_dmc/move_reports.sh</t>
+  </si>
+  <si>
+    <t>/tsys/prime/deployment/CREDIT/GLConv/backup/</t>
+  </si>
+  <si>
+    <t>/tsys/prime/deployment/CREDIT/directdebit/out/</t>
+  </si>
+  <si>
+    <t>/tsys/prime/deployment/CREDIT/directdebit/in/</t>
   </si>
 </sst>
 </file>
@@ -600,19 +600,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -620,13 +620,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E2" s="1"/>
     </row>
@@ -635,223 +635,223 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4" s="9"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E13" s="9"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E14" s="9"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E15" s="9"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E16" s="9"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E17" s="9"/>
     </row>
@@ -860,88 +860,88 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E18" s="9"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E19" s="9"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E20" s="9"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E21" s="9"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E22" s="9"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E23" s="9"/>
     </row>

</xml_diff>

<commit_message>
Code Version 190520 15:01
</commit_message>
<xml_diff>
--- a/Prime_Job_Automation/Configuration/Lookups/PostBatchScriptFileLocation.xlsx
+++ b/Prime_Job_Automation/Configuration/Lookups/PostBatchScriptFileLocation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\PJA\Prime_Job_Automation\Configuration\Lookups\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15AC5643-976D-43F2-96A1-065ED2E62921}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1DCAB9C-287B-4895-8CAD-27E5578C9E0D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,9 +32,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="51">
   <si>
-    <t>IsFolder?</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
@@ -50,9 +47,6 @@
     <t>/tsys/prime/deployment/CREDIT/Emboss/Work/runEmboss.com</t>
   </si>
   <si>
-    <t>IsExist?</t>
-  </si>
-  <si>
     <t>TSYSDW</t>
   </si>
   <si>
@@ -146,9 +140,6 @@
     <t>/home/pmuser01/check_reports.com</t>
   </si>
   <si>
-    <t>/prime/UBP_ubp/datawarehouse_file/EDS_TRANSFER//TSYS_DW.sh</t>
-  </si>
-  <si>
     <t>/prime/UBP_ubp/interfaces_outgoing/</t>
   </si>
   <si>
@@ -183,6 +174,15 @@
   </si>
   <si>
     <t>/tsys/prime/deployment/CREDIT/directdebit/in/</t>
+  </si>
+  <si>
+    <t>IsFolder</t>
+  </si>
+  <si>
+    <t>IsExist</t>
+  </si>
+  <si>
+    <t>/tsys/prime/UBP_ubp/datawarehouse_file/EDS_TRANSFER/TSYS_DW.sh</t>
   </si>
 </sst>
 </file>
@@ -600,19 +600,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>6</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -620,13 +620,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2" s="1"/>
     </row>
@@ -635,13 +635,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" s="1"/>
     </row>
@@ -650,13 +650,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" s="9"/>
     </row>
@@ -665,13 +665,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E5" s="1"/>
     </row>
@@ -680,13 +680,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E6" s="1"/>
     </row>
@@ -695,13 +695,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E7" s="1"/>
     </row>
@@ -710,13 +710,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E8" s="1"/>
     </row>
@@ -725,13 +725,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E9" s="1"/>
     </row>
@@ -740,13 +740,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10" s="1"/>
     </row>
@@ -755,13 +755,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E11" s="1"/>
     </row>
@@ -770,13 +770,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12" s="1"/>
     </row>
@@ -785,13 +785,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E13" s="9"/>
     </row>
@@ -800,13 +800,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E14" s="9"/>
     </row>
@@ -815,13 +815,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E15" s="9"/>
     </row>
@@ -830,13 +830,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E16" s="9"/>
     </row>
@@ -845,13 +845,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E17" s="9"/>
     </row>
@@ -860,13 +860,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E18" s="9"/>
     </row>
@@ -875,13 +875,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E19" s="9"/>
     </row>
@@ -890,13 +890,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E20" s="9"/>
     </row>
@@ -905,13 +905,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E21" s="9"/>
     </row>
@@ -920,13 +920,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E22" s="9"/>
     </row>
@@ -935,13 +935,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E23" s="9"/>
     </row>

</xml_diff>

<commit_message>
Code Version 190520 23:41
</commit_message>
<xml_diff>
--- a/Prime_Job_Automation/Configuration/Lookups/PostBatchScriptFileLocation.xlsx
+++ b/Prime_Job_Automation/Configuration/Lookups/PostBatchScriptFileLocation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\PJA\Prime_Job_Automation\Configuration\Lookups\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1DCAB9C-287B-4895-8CAD-27E5578C9E0D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4AA3CFF-9D1F-40EE-8A3C-CFDD6B0B339D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="53">
   <si>
     <t>No</t>
   </si>
@@ -183,6 +183,12 @@
   </si>
   <si>
     <t>/tsys/prime/UBP_ubp/datawarehouse_file/EDS_TRANSFER/TSYS_DW.sh</t>
+  </si>
+  <si>
+    <t>ConvertorIn</t>
+  </si>
+  <si>
+    <t>/home/pmuser01/converters/convert_biller/in</t>
   </si>
 </sst>
 </file>
@@ -586,7 +592,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -945,6 +951,21 @@
       </c>
       <c r="E23" s="9"/>
     </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Code Version 24052020 20:22
</commit_message>
<xml_diff>
--- a/Prime_Job_Automation/Configuration/Lookups/PostBatchScriptFileLocation.xlsx
+++ b/Prime_Job_Automation/Configuration/Lookups/PostBatchScriptFileLocation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\PJA\Prime_Job_Automation\Configuration\Lookups\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4AA3CFF-9D1F-40EE-8A3C-CFDD6B0B339D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{214C0497-3A21-4BD6-8C8C-7C0439C2E561}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="86">
   <si>
     <t>No</t>
   </si>
@@ -47,87 +47,21 @@
     <t>/tsys/prime/deployment/CREDIT/Emboss/Work/runEmboss.com</t>
   </si>
   <si>
-    <t>TSYSDW</t>
-  </si>
-  <si>
-    <t>MVReports</t>
-  </si>
-  <si>
-    <t>GLConv</t>
-  </si>
-  <si>
-    <t>GLBackup</t>
-  </si>
-  <si>
-    <t>RunEmboss</t>
-  </si>
-  <si>
-    <t>DirectDebitIn</t>
-  </si>
-  <si>
-    <t>DirectDebitShell</t>
-  </si>
-  <si>
-    <t>DirectDebitOut</t>
-  </si>
-  <si>
-    <t>VisaVCF</t>
-  </si>
-  <si>
-    <t>GLCPROConv</t>
-  </si>
-  <si>
     <t>Activity_Name</t>
   </si>
   <si>
     <t>Path</t>
   </si>
   <si>
-    <t>InterfaceOutgoing</t>
-  </si>
-  <si>
-    <t>Reports</t>
-  </si>
-  <si>
-    <t>GLCurrDate</t>
-  </si>
-  <si>
-    <t>EmbossInput</t>
-  </si>
-  <si>
-    <t>NonEmbossOutput</t>
-  </si>
-  <si>
     <t>/tsys/prime/deployment/CREDIT/Emboss/Outputs/NonEmbossing/</t>
   </si>
   <si>
-    <t>EmbossOutput</t>
-  </si>
-  <si>
     <t>/tsys/prime/deployment/CREDIT/Emboss/Outputs/Embossing/</t>
   </si>
   <si>
-    <t>StatementFiles</t>
-  </si>
-  <si>
-    <t>HostDebitFiles</t>
-  </si>
-  <si>
-    <t>ChckReports</t>
-  </si>
-  <si>
-    <t>UBPEmbossFiles</t>
-  </si>
-  <si>
-    <t>CollectorOutgoing</t>
-  </si>
-  <si>
     <t>/tsys/prime/deployment/CREDIT/GLConv/</t>
   </si>
   <si>
-    <t>ConvertorOutput</t>
-  </si>
-  <si>
     <t>/home/pmuser01/converters/convert_biller/work/convert_output.com</t>
   </si>
   <si>
@@ -185,17 +119,182 @@
     <t>/tsys/prime/UBP_ubp/datawarehouse_file/EDS_TRANSFER/TSYS_DW.sh</t>
   </si>
   <si>
-    <t>ConvertorIn</t>
-  </si>
-  <si>
     <t>/home/pmuser01/converters/convert_biller/in</t>
+  </si>
+  <si>
+    <t>/custom/deployment/CREDIT/reports/reports.com</t>
+  </si>
+  <si>
+    <t>/custom/deployment/CREDIT/reports/out/</t>
+  </si>
+  <si>
+    <t>Server</t>
+  </si>
+  <si>
+    <t>TSYS</t>
+  </si>
+  <si>
+    <t>/apps/staging_dir/TSYS/</t>
+  </si>
+  <si>
+    <t>/custom/deployment/CREDIT/reports/amla/amla.com</t>
+  </si>
+  <si>
+    <t>/custom/deployment/CREDIT/reports/tsys009/tsys009.com</t>
+  </si>
+  <si>
+    <t>\\172.16.17.183\CPSCIT\TPROD\</t>
+  </si>
+  <si>
+    <t>Network</t>
+  </si>
+  <si>
+    <t>fd_TSYSDW</t>
+  </si>
+  <si>
+    <t>fl_TSYSDW</t>
+  </si>
+  <si>
+    <t>/tsys/prime/UBP_ubp/datawarehouse_file/EDS_TRANSFER/</t>
+  </si>
+  <si>
+    <t>fd_MoveReports</t>
+  </si>
+  <si>
+    <t>fl_MoveReports</t>
+  </si>
+  <si>
+    <t>/home/pmuser01/MOVE_Reports_dmc/</t>
+  </si>
+  <si>
+    <t>fd_CheckReports</t>
+  </si>
+  <si>
+    <t>fl_CheckReports</t>
+  </si>
+  <si>
+    <t>/home/pmuser01/</t>
+  </si>
+  <si>
+    <t>fd_InterfaceOutgoing</t>
+  </si>
+  <si>
+    <t>fd_CollectorOutgoing</t>
+  </si>
+  <si>
+    <t>fd_Reports</t>
+  </si>
+  <si>
+    <t>fd_GLConvertor</t>
+  </si>
+  <si>
+    <t>fd_GLOutput</t>
+  </si>
+  <si>
+    <t>fl_GLConvertor</t>
+  </si>
+  <si>
+    <t>fd_EmbossInput</t>
+  </si>
+  <si>
+    <t>fl_RunEmboss</t>
+  </si>
+  <si>
+    <t>fd_NonEmbossOutput</t>
+  </si>
+  <si>
+    <t>fd_EmbossOutput</t>
+  </si>
+  <si>
+    <t>fd_StatementFiles</t>
+  </si>
+  <si>
+    <t>fd_HostDebitFiles</t>
+  </si>
+  <si>
+    <t>fd_DirectDebitIn</t>
+  </si>
+  <si>
+    <t>fl_DirectDebit</t>
+  </si>
+  <si>
+    <t>fd_GLBackup</t>
+  </si>
+  <si>
+    <t>fd_EodEmbossFiles</t>
+  </si>
+  <si>
+    <t>fd_DirectDebitOut</t>
+  </si>
+  <si>
+    <t>fd_VisaVCF</t>
+  </si>
+  <si>
+    <t>fl_ConvertBiller</t>
+  </si>
+  <si>
+    <t>fd_ConvertBillerIn</t>
+  </si>
+  <si>
+    <t>fd_DailyReportOutput</t>
+  </si>
+  <si>
+    <t>fl_DailyReportConvertor</t>
+  </si>
+  <si>
+    <t>fd_AmlaConvertor</t>
+  </si>
+  <si>
+    <t>fl_AmlaConvertor</t>
+  </si>
+  <si>
+    <t>fl_MonthlyReportConvertor</t>
+  </si>
+  <si>
+    <t>fd_MonthlyReportsOutput</t>
+  </si>
+  <si>
+    <t>/tsys/prime/deployment/CREDIT/Emboss/Work/</t>
+  </si>
+  <si>
+    <t>fd_RunEmboss</t>
+  </si>
+  <si>
+    <t>/tsys/prime/deployment/CREDIT/directdebit/work/</t>
+  </si>
+  <si>
+    <t>fd_DirectDebit</t>
+  </si>
+  <si>
+    <t>fd_ConvertBiller</t>
+  </si>
+  <si>
+    <t>/home/pmuser01/converters/convert_biller/work/</t>
+  </si>
+  <si>
+    <t>fd_DailyReportConvertor</t>
+  </si>
+  <si>
+    <t>/custom/deployment/CREDIT/reports/</t>
+  </si>
+  <si>
+    <t>/custom/deployment/CREDIT/reports/amla/</t>
+  </si>
+  <si>
+    <t>fd_MonthlyReportConvertor</t>
+  </si>
+  <si>
+    <t>/custom/deployment/CREDIT/reports/tsys009/</t>
+  </si>
+  <si>
+    <t>fd_AmlaStaging</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -214,6 +313,13 @@
       <b/>
       <sz val="10"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -260,7 +366,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -278,6 +384,10 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -338,7 +448,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -390,7 +500,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -592,382 +702,728 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="85.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>35</v>
+        <v>42</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>44</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E4" s="9"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>37</v>
+        <v>45</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>47</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E6" s="9"/>
+      <c r="F6" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>38</v>
+        <v>46</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>13</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="E7" s="9"/>
+      <c r="F7" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>2</v>
+        <v>50</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>33</v>
+        <v>51</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>4</v>
+      <c r="B12" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>22</v>
+        <v>53</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>2</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E13" s="9"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>24</v>
+        <v>54</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E14" s="9"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E14" s="1"/>
+      <c r="F14" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>40</v>
+      <c r="B15" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>74</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E15" s="9"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E15" s="1"/>
+      <c r="F15" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>41</v>
+      <c r="B16" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>4</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E16" s="9"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="E16" s="1"/>
+      <c r="F16" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>47</v>
+        <v>7</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E17" s="9"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>11</v>
+        <v>57</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E18" s="9"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>8</v>
+        <v>58</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E19" s="9"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="D20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E20" s="9"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="D21" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E21" s="9"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>13</v>
+        <v>77</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="D22" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E22" s="9"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E23" s="9"/>
+      <c r="F23" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24" s="9"/>
+      <c r="F24" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" s="9"/>
+      <c r="F25" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E26" s="9"/>
+      <c r="F26" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E27" s="9"/>
+      <c r="F27" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E28" s="9"/>
+      <c r="F28" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E29" s="9"/>
+      <c r="F29" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>29</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E30" s="1"/>
+      <c r="F30" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>30</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E31" s="1"/>
+      <c r="F31" s="12">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
         <v>31</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="B32" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E32" s="1"/>
+      <c r="F32" s="12">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
         <v>32</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="B33" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E33" s="1"/>
+      <c r="F33" s="12">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>33</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E34" s="1"/>
+      <c r="F34" s="12">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>34</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E35" s="1"/>
+      <c r="F35" s="12">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>35</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E23" s="9"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
-        <v>23</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E24" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="12">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>36</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E37" s="1"/>
+      <c r="F37" s="12">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>37</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E38" s="1"/>
+      <c r="F38" s="12">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>38</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1" t="s">
+        <v>38</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C39" r:id="rId1" xr:uid="{2E562633-CC59-4AC3-9EC2-1C192113452B}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Code Version 28052020 0103
</commit_message>
<xml_diff>
--- a/Prime_Job_Automation/Configuration/Lookups/PostBatchScriptFileLocation.xlsx
+++ b/Prime_Job_Automation/Configuration/Lookups/PostBatchScriptFileLocation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\PJA\Prime_Job_Automation\Configuration\Lookups\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{214C0497-3A21-4BD6-8C8C-7C0439C2E561}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D765E0D-6E53-44CE-92CC-CEF9A8742A7B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="91">
   <si>
     <t>No</t>
   </si>
@@ -38,9 +38,6 @@
     <t>S.No</t>
   </si>
   <si>
-    <t>/tsys/prime/deployment/CREDIT/GLConv/GLCPROConv.com</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -62,9 +59,6 @@
     <t>/tsys/prime/deployment/CREDIT/GLConv/</t>
   </si>
   <si>
-    <t>/home/pmuser01/converters/convert_biller/work/convert_output.com</t>
-  </si>
-  <si>
     <t>/tsys/prime/deployment/CREDIT/Emboss/Inputs/</t>
   </si>
   <si>
@@ -119,9 +113,6 @@
     <t>/tsys/prime/UBP_ubp/datawarehouse_file/EDS_TRANSFER/TSYS_DW.sh</t>
   </si>
   <si>
-    <t>/home/pmuser01/converters/convert_biller/in</t>
-  </si>
-  <si>
     <t>/custom/deployment/CREDIT/reports/reports.com</t>
   </si>
   <si>
@@ -131,21 +122,12 @@
     <t>Server</t>
   </si>
   <si>
-    <t>TSYS</t>
-  </si>
-  <si>
-    <t>/apps/staging_dir/TSYS/</t>
-  </si>
-  <si>
     <t>/custom/deployment/CREDIT/reports/amla/amla.com</t>
   </si>
   <si>
     <t>/custom/deployment/CREDIT/reports/tsys009/tsys009.com</t>
   </si>
   <si>
-    <t>\\172.16.17.183\CPSCIT\TPROD\</t>
-  </si>
-  <si>
     <t>Network</t>
   </si>
   <si>
@@ -269,9 +251,6 @@
     <t>fd_ConvertBiller</t>
   </si>
   <si>
-    <t>/home/pmuser01/converters/convert_biller/work/</t>
-  </si>
-  <si>
     <t>fd_DailyReportConvertor</t>
   </si>
   <si>
@@ -288,6 +267,42 @@
   </si>
   <si>
     <t>fd_AmlaStaging</t>
+  </si>
+  <si>
+    <t>TSYSApp</t>
+  </si>
+  <si>
+    <t>TSysDB</t>
+  </si>
+  <si>
+    <t>AMLA</t>
+  </si>
+  <si>
+    <t>UBIX</t>
+  </si>
+  <si>
+    <t>fd_UBIX</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>/tsys/prime/deployment/CREDIT/GLConv/GLCPROConv1.com</t>
+  </si>
+  <si>
+    <t>/tsys/prime/deployment/CREDIT/convert_biller/work/</t>
+  </si>
+  <si>
+    <t>/tsys/prime/deployment/CREDIT/convert_biller/work/convert_output.com</t>
+  </si>
+  <si>
+    <t>/tsys/prime/deployment/CREDIT/convert_biller/in/</t>
+  </si>
+  <si>
+    <t>/prime/apps/staging_dir/TSYS/</t>
+  </si>
+  <si>
+    <t>\\10.19.81.248\rpa\PMU\CPSCIT\TPROD</t>
   </si>
 </sst>
 </file>
@@ -448,7 +463,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -500,7 +515,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -702,7 +717,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -720,19 +735,19 @@
         <v>1</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>6</v>
-      </c>
       <c r="D1" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -740,17 +755,17 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="11" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -758,17 +773,17 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="11" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -776,17 +791,17 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="11" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -794,17 +809,17 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="11" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -812,17 +827,17 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E6" s="9"/>
       <c r="F6" s="11" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -830,17 +845,17 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="11" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -848,17 +863,17 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="11" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -866,17 +881,17 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="11" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -884,17 +899,17 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="11" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -902,17 +917,17 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="11" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -920,17 +935,17 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="11" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -938,17 +953,17 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>2</v>
+        <v>85</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="11" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -956,17 +971,17 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="11" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -974,17 +989,17 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="11" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -992,17 +1007,17 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="11" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1010,17 +1025,17 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E17" s="9"/>
       <c r="F17" s="11" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1028,17 +1043,17 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E18" s="9"/>
       <c r="F18" s="11" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1046,17 +1061,17 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E19" s="9"/>
       <c r="F19" s="11" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1064,17 +1079,17 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E20" s="9"/>
       <c r="F20" s="11" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1082,17 +1097,17 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E21" s="9"/>
       <c r="F21" s="11" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1100,17 +1115,17 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E22" s="9"/>
       <c r="F22" s="11" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1118,17 +1133,17 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E23" s="9"/>
       <c r="F23" s="11" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1136,17 +1151,17 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E24" s="9"/>
       <c r="F24" s="11" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1154,17 +1169,17 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E25" s="9"/>
       <c r="F25" s="11" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1172,17 +1187,17 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E26" s="9"/>
       <c r="F26" s="11" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1190,17 +1205,17 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E27" s="9"/>
       <c r="F27" s="11" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1208,17 +1223,17 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E28" s="9"/>
       <c r="F28" s="11" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1226,17 +1241,17 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E29" s="9"/>
       <c r="F29" s="11" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1244,17 +1259,17 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>29</v>
+        <v>88</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="11" t="s">
-        <v>33</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1262,17 +1277,17 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E31" s="1"/>
-      <c r="F31" s="12">
-        <v>108</v>
+      <c r="F31" s="11" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1280,17 +1295,17 @@
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E32" s="1"/>
-      <c r="F32" s="12">
-        <v>108</v>
+      <c r="F32" s="11" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1298,17 +1313,17 @@
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E33" s="1"/>
-      <c r="F33" s="12">
-        <v>108</v>
+      <c r="F33" s="11" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1316,17 +1331,17 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>34</v>
+        <v>89</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E34" s="1"/>
-      <c r="F34" s="12">
-        <v>83</v>
+      <c r="F34" s="12" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1334,17 +1349,17 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E35" s="1"/>
-      <c r="F35" s="12">
-        <v>108</v>
+      <c r="F35" s="11" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1352,17 +1367,17 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E36" s="1"/>
-      <c r="F36" s="12">
-        <v>108</v>
+      <c r="F36" s="11" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -1370,17 +1385,17 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E37" s="1"/>
-      <c r="F37" s="12">
-        <v>108</v>
+      <c r="F37" s="11" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -1388,17 +1403,17 @@
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E38" s="1"/>
-      <c r="F38" s="12">
-        <v>108</v>
+      <c r="F38" s="11" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -1406,22 +1421,40 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>37</v>
+        <v>90</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E39" s="1"/>
       <c r="F39" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="9">
+        <v>39</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C39" r:id="rId1" xr:uid="{2E562633-CC59-4AC3-9EC2-1C192113452B}"/>
+    <hyperlink ref="C39" r:id="rId1" display="\\172.16.17.183\CPSCIT\TPROD\" xr:uid="{2E562633-CC59-4AC3-9EC2-1C192113452B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
Code Version 29052020 1333
</commit_message>
<xml_diff>
--- a/Prime_Job_Automation/Configuration/Lookups/PostBatchScriptFileLocation.xlsx
+++ b/Prime_Job_Automation/Configuration/Lookups/PostBatchScriptFileLocation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\PJA\Prime_Job_Automation\Configuration\Lookups\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D765E0D-6E53-44CE-92CC-CEF9A8742A7B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{773619A5-0B45-416E-990F-48FC5E134595}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="95">
   <si>
     <t>No</t>
   </si>
@@ -303,6 +303,18 @@
   </si>
   <si>
     <t>\\10.19.81.248\rpa\PMU\CPSCIT\TPROD</t>
+  </si>
+  <si>
+    <t>\\172.16.17.183\pmu\emboss_files\TSYSCREDIT\embossing</t>
+  </si>
+  <si>
+    <t>\\172.16.17.183\pmu\emboss_files\TSYSCREDIT\non_embossing</t>
+  </si>
+  <si>
+    <t>fd_NonEmbossingPcidssFolder</t>
+  </si>
+  <si>
+    <t>fd_EmbossingPcidssFolder</t>
   </si>
 </sst>
 </file>
@@ -717,14 +729,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="85.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1"/>
@@ -1452,11 +1464,49 @@
         <v>82</v>
       </c>
     </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="9">
+        <v>40</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="9">
+        <v>41</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C39" r:id="rId1" display="\\172.16.17.183\CPSCIT\TPROD\" xr:uid="{2E562633-CC59-4AC3-9EC2-1C192113452B}"/>
+    <hyperlink ref="C41" r:id="rId2" xr:uid="{FBB1FA95-E234-49DF-A127-F678C42A6949}"/>
+    <hyperlink ref="C42" r:id="rId3" xr:uid="{B73E96E8-9834-49FF-9A12-708E47593BC7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>